<commit_message>
Hyundai data ETL automation. Added the sample data to use
</commit_message>
<xml_diff>
--- a/landing_zone/2026/Honda/2025-06/2026_Honda_Accessories-06-2025.xlsx
+++ b/landing_zone/2026/Honda/2025-06/2026_Honda_Accessories-06-2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pbssystems-my.sharepoint.com/personal/paxm_pbssystems_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pbssystems-my.sharepoint.com/personal/paxm_pbssystems_com/Documents/Desktop/Office/Projects/OEM Accessory project/OEM Accessories_v1/landing_zone/2026/Honda/2025-06/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="814" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FED45004-B4C1-46C8-98DB-F9D8F13C8FD0}"/>
+  <xr:revisionPtr revIDLastSave="818" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{986A5247-C35B-426E-96E0-CEB87B4C737E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master Upload - HRV " sheetId="22" r:id="rId1"/>
@@ -34161,7 +34161,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35820,7 +35820,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35861,155 +35861,155 @@
       <c r="A2" t="s">
         <v>490</v>
       </c>
-      <c r="B2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D2" t="s">
-        <v>256</v>
-      </c>
-      <c r="E2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" t="s">
-        <v>257</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>527</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>528</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>528</v>
+      </c>
+      <c r="G2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>490</v>
       </c>
       <c r="B3" t="s">
-        <v>259</v>
+        <v>282</v>
+      </c>
+      <c r="C3" t="s">
+        <v>283</v>
       </c>
       <c r="D3" t="s">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>247</v>
       </c>
       <c r="F3" t="s">
-        <v>261</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+      <c r="G3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>490</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>287</v>
       </c>
       <c r="C4" t="s">
-        <v>263</v>
+        <v>288</v>
       </c>
       <c r="D4" t="s">
-        <v>264</v>
+        <v>284</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>247</v>
       </c>
       <c r="F4" t="s">
-        <v>265</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+      <c r="G4" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>490</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="D5" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="E5" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="F5" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>490</v>
       </c>
       <c r="B6" t="s">
-        <v>271</v>
-      </c>
-      <c r="C6" t="s">
-        <v>272</v>
+        <v>259</v>
       </c>
       <c r="D6" t="s">
-        <v>273</v>
+        <v>260</v>
       </c>
       <c r="E6" t="s">
-        <v>274</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>490</v>
       </c>
       <c r="B7" t="s">
-        <v>491</v>
+        <v>289</v>
       </c>
       <c r="C7" t="s">
-        <v>492</v>
+        <v>290</v>
       </c>
       <c r="D7" t="s">
-        <v>128</v>
+        <v>291</v>
       </c>
       <c r="E7" t="s">
-        <v>313</v>
+        <v>247</v>
       </c>
       <c r="F7" t="s">
-        <v>493</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="G7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>490</v>
       </c>
       <c r="B8" t="s">
-        <v>495</v>
+        <v>293</v>
       </c>
       <c r="C8" t="s">
-        <v>496</v>
+        <v>294</v>
       </c>
       <c r="D8" t="s">
-        <v>497</v>
+        <v>295</v>
       </c>
       <c r="E8" t="s">
-        <v>498</v>
+        <v>247</v>
       </c>
       <c r="F8" t="s">
-        <v>499</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>500</v>
+        <v>296</v>
+      </c>
+      <c r="G8" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -36017,19 +36017,19 @@
         <v>490</v>
       </c>
       <c r="B9" t="s">
-        <v>282</v>
+        <v>297</v>
       </c>
       <c r="C9" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="D9" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="E9" t="s">
         <v>247</v>
       </c>
       <c r="F9" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="G9" t="s">
         <v>286</v>
@@ -36040,22 +36040,22 @@
         <v>490</v>
       </c>
       <c r="B10" t="s">
-        <v>287</v>
+        <v>520</v>
       </c>
       <c r="C10" t="s">
-        <v>288</v>
+        <v>521</v>
       </c>
       <c r="D10" t="s">
-        <v>284</v>
+        <v>522</v>
       </c>
       <c r="E10" t="s">
-        <v>247</v>
+        <v>142</v>
       </c>
       <c r="F10" t="s">
-        <v>285</v>
+        <v>522</v>
       </c>
       <c r="G10" t="s">
-        <v>286</v>
+        <v>515</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -36063,22 +36063,22 @@
         <v>490</v>
       </c>
       <c r="B11" t="s">
-        <v>289</v>
+        <v>523</v>
       </c>
       <c r="C11" t="s">
-        <v>290</v>
+        <v>524</v>
       </c>
       <c r="D11" t="s">
-        <v>291</v>
+        <v>525</v>
       </c>
       <c r="E11" t="s">
-        <v>247</v>
+        <v>142</v>
       </c>
       <c r="F11" t="s">
-        <v>292</v>
+        <v>525</v>
       </c>
       <c r="G11" t="s">
-        <v>286</v>
+        <v>515</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -36086,22 +36086,19 @@
         <v>490</v>
       </c>
       <c r="B12" t="s">
-        <v>293</v>
+        <v>168</v>
       </c>
       <c r="C12" t="s">
-        <v>294</v>
+        <v>387</v>
       </c>
       <c r="D12" t="s">
-        <v>295</v>
+        <v>388</v>
       </c>
       <c r="E12" t="s">
-        <v>247</v>
+        <v>172</v>
       </c>
       <c r="F12" t="s">
-        <v>296</v>
-      </c>
-      <c r="G12" t="s">
-        <v>286</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -36109,22 +36106,22 @@
         <v>490</v>
       </c>
       <c r="B13" t="s">
-        <v>297</v>
+        <v>516</v>
       </c>
       <c r="C13" t="s">
-        <v>298</v>
+        <v>517</v>
       </c>
       <c r="D13" t="s">
-        <v>295</v>
+        <v>518</v>
       </c>
       <c r="E13" t="s">
-        <v>247</v>
+        <v>88</v>
       </c>
       <c r="F13" t="s">
-        <v>296</v>
+        <v>519</v>
       </c>
       <c r="G13" t="s">
-        <v>286</v>
+        <v>515</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -36132,22 +36129,19 @@
         <v>490</v>
       </c>
       <c r="B14" t="s">
-        <v>299</v>
+        <v>323</v>
       </c>
       <c r="C14" t="s">
-        <v>300</v>
+        <v>324</v>
       </c>
       <c r="D14" t="s">
-        <v>301</v>
+        <v>325</v>
       </c>
       <c r="E14" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>302</v>
-      </c>
-      <c r="G14" t="s">
-        <v>303</v>
+        <v>326</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -36155,19 +36149,19 @@
         <v>490</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>183</v>
       </c>
       <c r="C15" t="s">
-        <v>304</v>
+        <v>394</v>
       </c>
       <c r="D15" t="s">
-        <v>305</v>
+        <v>395</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="F15" t="s">
-        <v>306</v>
+        <v>396</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -36175,19 +36169,19 @@
         <v>490</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>195</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>408</v>
       </c>
       <c r="D16" t="s">
-        <v>29</v>
+        <v>341</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
+        <v>409</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -36195,19 +36189,19 @@
         <v>490</v>
       </c>
       <c r="B17" t="s">
-        <v>501</v>
+        <v>410</v>
       </c>
       <c r="C17" t="s">
-        <v>502</v>
+        <v>411</v>
       </c>
       <c r="D17" t="s">
-        <v>503</v>
+        <v>412</v>
       </c>
       <c r="E17" t="s">
-        <v>313</v>
+        <v>172</v>
       </c>
       <c r="F17" t="s">
-        <v>504</v>
+        <v>413</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -36215,19 +36209,22 @@
         <v>490</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>424</v>
       </c>
       <c r="C18" t="s">
-        <v>307</v>
+        <v>508</v>
       </c>
       <c r="D18" t="s">
-        <v>308</v>
+        <v>509</v>
       </c>
       <c r="E18" t="s">
         <v>19</v>
       </c>
       <c r="F18" t="s">
-        <v>309</v>
+        <v>510</v>
+      </c>
+      <c r="G18" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -36235,19 +36232,19 @@
         <v>490</v>
       </c>
       <c r="B19" t="s">
-        <v>310</v>
+        <v>179</v>
       </c>
       <c r="C19" t="s">
-        <v>311</v>
+        <v>506</v>
       </c>
       <c r="D19" t="s">
-        <v>312</v>
+        <v>391</v>
       </c>
       <c r="E19" t="s">
-        <v>313</v>
+        <v>172</v>
       </c>
       <c r="F19" t="s">
-        <v>314</v>
+        <v>392</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -36255,22 +36252,22 @@
         <v>490</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>372</v>
       </c>
       <c r="C20" t="s">
-        <v>315</v>
+        <v>373</v>
       </c>
       <c r="D20" t="s">
-        <v>316</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="F20" t="s">
-        <v>317</v>
+        <v>374</v>
       </c>
       <c r="G20" t="s">
-        <v>318</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -36278,19 +36275,19 @@
         <v>490</v>
       </c>
       <c r="B21" t="s">
-        <v>319</v>
+        <v>153</v>
       </c>
       <c r="C21" t="s">
-        <v>320</v>
+        <v>382</v>
       </c>
       <c r="D21" t="s">
-        <v>321</v>
+        <v>380</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F21" t="s">
-        <v>322</v>
+        <v>381</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -36298,19 +36295,19 @@
         <v>490</v>
       </c>
       <c r="B22" t="s">
-        <v>323</v>
+        <v>153</v>
       </c>
       <c r="C22" t="s">
-        <v>324</v>
+        <v>444</v>
       </c>
       <c r="D22" t="s">
-        <v>325</v>
+        <v>442</v>
       </c>
       <c r="E22" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>326</v>
+        <v>443</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -36318,22 +36315,19 @@
         <v>490</v>
       </c>
       <c r="B23" t="s">
-        <v>95</v>
+        <v>153</v>
       </c>
       <c r="C23" t="s">
-        <v>331</v>
+        <v>217</v>
       </c>
       <c r="D23" t="s">
-        <v>332</v>
+        <v>447</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>142</v>
       </c>
       <c r="F23" t="s">
-        <v>333</v>
-      </c>
-      <c r="G23" t="s">
-        <v>334</v>
+        <v>447</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -36341,19 +36335,22 @@
         <v>490</v>
       </c>
       <c r="B24" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C24" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="D24" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="E24" t="s">
         <v>76</v>
       </c>
       <c r="F24" t="s">
-        <v>338</v>
+        <v>342</v>
+      </c>
+      <c r="G24" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -36361,22 +36358,19 @@
         <v>490</v>
       </c>
       <c r="B25" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="C25" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D25" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E25" t="s">
         <v>76</v>
       </c>
       <c r="F25" t="s">
-        <v>342</v>
-      </c>
-      <c r="G25" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -36384,19 +36378,22 @@
         <v>490</v>
       </c>
       <c r="B26" t="s">
-        <v>344</v>
+        <v>191</v>
       </c>
       <c r="C26" t="s">
-        <v>345</v>
+        <v>400</v>
       </c>
       <c r="D26" t="s">
-        <v>346</v>
+        <v>401</v>
       </c>
       <c r="E26" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="F26" t="s">
-        <v>347</v>
+        <v>402</v>
+      </c>
+      <c r="G26" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -36424,19 +36421,22 @@
         <v>490</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>351</v>
+        <v>315</v>
       </c>
       <c r="D28" t="s">
-        <v>132</v>
+        <v>316</v>
       </c>
       <c r="E28" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="F28" t="s">
-        <v>352</v>
+        <v>317</v>
+      </c>
+      <c r="G28" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -36444,19 +36444,22 @@
         <v>490</v>
       </c>
       <c r="B29" t="s">
-        <v>143</v>
+        <v>220</v>
       </c>
       <c r="C29" t="s">
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="D29" t="s">
-        <v>145</v>
+        <v>222</v>
       </c>
       <c r="E29" t="s">
         <v>142</v>
       </c>
       <c r="F29" t="s">
-        <v>145</v>
+        <v>222</v>
+      </c>
+      <c r="G29" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -36464,22 +36467,22 @@
         <v>490</v>
       </c>
       <c r="B30" t="s">
-        <v>353</v>
+        <v>224</v>
       </c>
       <c r="C30" t="s">
-        <v>354</v>
+        <v>225</v>
       </c>
       <c r="D30" t="s">
-        <v>355</v>
+        <v>450</v>
       </c>
       <c r="E30" t="s">
-        <v>60</v>
+        <v>142</v>
       </c>
       <c r="F30" t="s">
-        <v>356</v>
+        <v>450</v>
       </c>
       <c r="G30" t="s">
-        <v>357</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -36487,19 +36490,19 @@
         <v>490</v>
       </c>
       <c r="B31" t="s">
-        <v>358</v>
+        <v>319</v>
       </c>
       <c r="C31" t="s">
-        <v>359</v>
+        <v>320</v>
       </c>
       <c r="D31" t="s">
-        <v>360</v>
+        <v>321</v>
       </c>
       <c r="E31" t="s">
-        <v>361</v>
+        <v>13</v>
       </c>
       <c r="F31" t="s">
-        <v>362</v>
+        <v>322</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -36507,19 +36510,19 @@
         <v>490</v>
       </c>
       <c r="B32" t="s">
-        <v>363</v>
+        <v>501</v>
       </c>
       <c r="C32" t="s">
-        <v>364</v>
+        <v>502</v>
       </c>
       <c r="D32" t="s">
-        <v>365</v>
+        <v>503</v>
       </c>
       <c r="E32" t="s">
-        <v>142</v>
+        <v>313</v>
       </c>
       <c r="F32" t="s">
-        <v>365</v>
+        <v>504</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -36527,19 +36530,19 @@
         <v>490</v>
       </c>
       <c r="B33" t="s">
-        <v>366</v>
+        <v>143</v>
       </c>
       <c r="C33" t="s">
-        <v>367</v>
+        <v>144</v>
       </c>
       <c r="D33" t="s">
-        <v>365</v>
+        <v>145</v>
       </c>
       <c r="E33" t="s">
         <v>142</v>
       </c>
       <c r="F33" t="s">
-        <v>365</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -36547,19 +36550,19 @@
         <v>490</v>
       </c>
       <c r="B34" t="s">
-        <v>368</v>
+        <v>427</v>
       </c>
       <c r="C34" t="s">
-        <v>369</v>
+        <v>428</v>
       </c>
       <c r="D34" t="s">
-        <v>370</v>
+        <v>429</v>
       </c>
       <c r="E34" t="s">
-        <v>94</v>
+        <v>430</v>
       </c>
       <c r="F34" t="s">
-        <v>371</v>
+        <v>431</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -36567,22 +36570,19 @@
         <v>490</v>
       </c>
       <c r="B35" t="s">
-        <v>372</v>
+        <v>344</v>
       </c>
       <c r="C35" t="s">
-        <v>373</v>
+        <v>345</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>346</v>
       </c>
       <c r="E35" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="F35" t="s">
-        <v>374</v>
-      </c>
-      <c r="G35" t="s">
-        <v>375</v>
+        <v>347</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -36590,19 +36590,22 @@
         <v>490</v>
       </c>
       <c r="B36" t="s">
-        <v>126</v>
+        <v>419</v>
       </c>
       <c r="C36" t="s">
-        <v>127</v>
+        <v>420</v>
       </c>
       <c r="D36" t="s">
-        <v>128</v>
+        <v>421</v>
       </c>
       <c r="E36" t="s">
-        <v>13</v>
+        <v>313</v>
       </c>
       <c r="F36" t="s">
-        <v>129</v>
+        <v>422</v>
+      </c>
+      <c r="G36" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -36610,39 +36613,45 @@
         <v>490</v>
       </c>
       <c r="B37" t="s">
-        <v>130</v>
+        <v>511</v>
       </c>
       <c r="C37" t="s">
-        <v>131</v>
+        <v>512</v>
       </c>
       <c r="D37" t="s">
-        <v>132</v>
+        <v>513</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="F37" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>514</v>
+      </c>
+      <c r="G37" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>490</v>
       </c>
       <c r="B38" t="s">
-        <v>377</v>
+        <v>491</v>
       </c>
       <c r="C38" t="s">
-        <v>110</v>
+        <v>492</v>
       </c>
       <c r="D38" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="E38" t="s">
-        <v>19</v>
+        <v>313</v>
       </c>
       <c r="F38" t="s">
-        <v>112</v>
+        <v>493</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -36650,19 +36659,22 @@
         <v>490</v>
       </c>
       <c r="B39" t="s">
-        <v>122</v>
+        <v>491</v>
       </c>
       <c r="C39" t="s">
-        <v>123</v>
+        <v>492</v>
       </c>
       <c r="D39" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="E39" t="s">
-        <v>13</v>
+        <v>313</v>
       </c>
       <c r="F39" t="s">
-        <v>125</v>
+        <v>493</v>
+      </c>
+      <c r="G39" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -36670,19 +36682,22 @@
         <v>490</v>
       </c>
       <c r="B40" t="s">
-        <v>118</v>
+        <v>414</v>
       </c>
       <c r="C40" t="s">
-        <v>119</v>
+        <v>415</v>
       </c>
       <c r="D40" t="s">
-        <v>378</v>
+        <v>416</v>
       </c>
       <c r="E40" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="F40" t="s">
-        <v>121</v>
+        <v>417</v>
+      </c>
+      <c r="G40" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -36690,19 +36705,19 @@
         <v>490</v>
       </c>
       <c r="B41" t="s">
-        <v>134</v>
+        <v>72</v>
       </c>
       <c r="C41" t="s">
-        <v>135</v>
+        <v>307</v>
       </c>
       <c r="D41" t="s">
-        <v>136</v>
+        <v>308</v>
       </c>
       <c r="E41" t="s">
-        <v>76</v>
+        <v>19</v>
       </c>
       <c r="F41" t="s">
-        <v>137</v>
+        <v>309</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -36710,10 +36725,10 @@
         <v>490</v>
       </c>
       <c r="B42" t="s">
-        <v>146</v>
+        <v>476</v>
       </c>
       <c r="C42" t="s">
-        <v>379</v>
+        <v>480</v>
       </c>
       <c r="D42" t="s">
         <v>380</v>
@@ -36730,19 +36745,19 @@
         <v>490</v>
       </c>
       <c r="B43" t="s">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="C43" t="s">
-        <v>469</v>
+        <v>477</v>
       </c>
       <c r="D43" t="s">
-        <v>380</v>
+        <v>442</v>
       </c>
       <c r="E43" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="F43" t="s">
-        <v>381</v>
+        <v>443</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -36753,16 +36768,16 @@
         <v>476</v>
       </c>
       <c r="C44" t="s">
-        <v>480</v>
+        <v>529</v>
       </c>
       <c r="D44" t="s">
-        <v>380</v>
+        <v>447</v>
       </c>
       <c r="E44" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="F44" t="s">
-        <v>381</v>
+        <v>447</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -36770,19 +36785,19 @@
         <v>490</v>
       </c>
       <c r="B45" t="s">
-        <v>153</v>
+        <v>84</v>
       </c>
       <c r="C45" t="s">
-        <v>382</v>
+        <v>351</v>
       </c>
       <c r="D45" t="s">
-        <v>380</v>
+        <v>132</v>
       </c>
       <c r="E45" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="F45" t="s">
-        <v>381</v>
+        <v>352</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -36790,19 +36805,19 @@
         <v>490</v>
       </c>
       <c r="B46" t="s">
-        <v>383</v>
+        <v>206</v>
       </c>
       <c r="C46" t="s">
-        <v>384</v>
+        <v>207</v>
       </c>
       <c r="D46" t="s">
-        <v>380</v>
+        <v>435</v>
       </c>
       <c r="E46" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="F46" t="s">
-        <v>381</v>
+        <v>435</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -36810,19 +36825,19 @@
         <v>490</v>
       </c>
       <c r="B47" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
       <c r="C47" t="s">
-        <v>387</v>
+        <v>210</v>
       </c>
       <c r="D47" t="s">
-        <v>388</v>
+        <v>141</v>
       </c>
       <c r="E47" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="F47" t="s">
-        <v>389</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -36830,19 +36845,22 @@
         <v>490</v>
       </c>
       <c r="B48" t="s">
-        <v>179</v>
+        <v>227</v>
       </c>
       <c r="C48" t="s">
-        <v>506</v>
+        <v>228</v>
       </c>
       <c r="D48" t="s">
-        <v>391</v>
+        <v>451</v>
       </c>
       <c r="E48" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="F48" t="s">
-        <v>392</v>
+        <v>451</v>
+      </c>
+      <c r="G48" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -36850,19 +36868,19 @@
         <v>490</v>
       </c>
       <c r="B49" t="s">
-        <v>183</v>
+        <v>436</v>
       </c>
       <c r="C49" t="s">
-        <v>394</v>
+        <v>474</v>
       </c>
       <c r="D49" t="s">
-        <v>395</v>
+        <v>438</v>
       </c>
       <c r="E49" t="s">
-        <v>172</v>
+        <v>439</v>
       </c>
       <c r="F49" t="s">
-        <v>396</v>
+        <v>440</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -36870,19 +36888,19 @@
         <v>490</v>
       </c>
       <c r="B50" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
       <c r="C50" t="s">
-        <v>507</v>
+        <v>379</v>
       </c>
       <c r="D50" t="s">
-        <v>398</v>
+        <v>380</v>
       </c>
       <c r="E50" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="F50" t="s">
-        <v>399</v>
+        <v>381</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -36890,22 +36908,19 @@
         <v>490</v>
       </c>
       <c r="B51" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="C51" t="s">
-        <v>400</v>
+        <v>441</v>
       </c>
       <c r="D51" t="s">
-        <v>401</v>
+        <v>442</v>
       </c>
       <c r="E51" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="F51" t="s">
-        <v>402</v>
-      </c>
-      <c r="G51" t="s">
-        <v>403</v>
+        <v>443</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -36913,59 +36928,65 @@
         <v>490</v>
       </c>
       <c r="B52" t="s">
-        <v>404</v>
+        <v>146</v>
       </c>
       <c r="C52" t="s">
-        <v>405</v>
+        <v>212</v>
       </c>
       <c r="D52" t="s">
-        <v>406</v>
+        <v>447</v>
       </c>
       <c r="E52" t="s">
-        <v>94</v>
+        <v>142</v>
       </c>
       <c r="F52" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>490</v>
       </c>
       <c r="B53" t="s">
-        <v>195</v>
+        <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>408</v>
+        <v>263</v>
       </c>
       <c r="D53" t="s">
-        <v>341</v>
+        <v>264</v>
       </c>
       <c r="E53" t="s">
-        <v>172</v>
+        <v>13</v>
       </c>
       <c r="F53" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>490</v>
       </c>
       <c r="B54" t="s">
-        <v>410</v>
+        <v>15</v>
       </c>
       <c r="C54" t="s">
-        <v>411</v>
+        <v>267</v>
       </c>
       <c r="D54" t="s">
-        <v>412</v>
+        <v>268</v>
       </c>
       <c r="E54" t="s">
-        <v>172</v>
+        <v>94</v>
       </c>
       <c r="F54" t="s">
-        <v>413</v>
+        <v>269</v>
+      </c>
+      <c r="G54" s="4" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -36973,22 +36994,19 @@
         <v>490</v>
       </c>
       <c r="B55" t="s">
-        <v>414</v>
+        <v>383</v>
       </c>
       <c r="C55" t="s">
-        <v>415</v>
+        <v>384</v>
       </c>
       <c r="D55" t="s">
-        <v>416</v>
+        <v>380</v>
       </c>
       <c r="E55" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F55" t="s">
-        <v>417</v>
-      </c>
-      <c r="G55" t="s">
-        <v>418</v>
+        <v>381</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -36996,22 +37014,19 @@
         <v>490</v>
       </c>
       <c r="B56" t="s">
-        <v>419</v>
+        <v>383</v>
       </c>
       <c r="C56" t="s">
-        <v>420</v>
+        <v>445</v>
       </c>
       <c r="D56" t="s">
-        <v>421</v>
+        <v>442</v>
       </c>
       <c r="E56" t="s">
-        <v>313</v>
+        <v>25</v>
       </c>
       <c r="F56" t="s">
-        <v>422</v>
-      </c>
-      <c r="G56" t="s">
-        <v>423</v>
+        <v>443</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -37019,22 +37034,19 @@
         <v>490</v>
       </c>
       <c r="B57" t="s">
-        <v>424</v>
+        <v>383</v>
       </c>
       <c r="C57" t="s">
-        <v>508</v>
+        <v>448</v>
       </c>
       <c r="D57" t="s">
-        <v>509</v>
+        <v>447</v>
       </c>
       <c r="E57" t="s">
-        <v>19</v>
+        <v>142</v>
       </c>
       <c r="F57" t="s">
-        <v>510</v>
-      </c>
-      <c r="G57" t="s">
-        <v>418</v>
+        <v>447</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -37042,19 +37054,19 @@
         <v>490</v>
       </c>
       <c r="B58" t="s">
-        <v>427</v>
+        <v>187</v>
       </c>
       <c r="C58" t="s">
-        <v>428</v>
+        <v>507</v>
       </c>
       <c r="D58" t="s">
-        <v>429</v>
+        <v>398</v>
       </c>
       <c r="E58" t="s">
-        <v>430</v>
+        <v>13</v>
       </c>
       <c r="F58" t="s">
-        <v>431</v>
+        <v>399</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -37062,19 +37074,19 @@
         <v>490</v>
       </c>
       <c r="B59" t="s">
-        <v>206</v>
+        <v>134</v>
       </c>
       <c r="C59" t="s">
-        <v>207</v>
+        <v>135</v>
       </c>
       <c r="D59" t="s">
-        <v>435</v>
+        <v>136</v>
       </c>
       <c r="E59" t="s">
-        <v>142</v>
+        <v>76</v>
       </c>
       <c r="F59" t="s">
-        <v>435</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -37082,19 +37094,19 @@
         <v>490</v>
       </c>
       <c r="B60" t="s">
-        <v>209</v>
+        <v>377</v>
       </c>
       <c r="C60" t="s">
-        <v>210</v>
+        <v>110</v>
       </c>
       <c r="D60" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
       <c r="E60" t="s">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="F60" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -37102,22 +37114,19 @@
         <v>490</v>
       </c>
       <c r="B61" t="s">
-        <v>511</v>
+        <v>118</v>
       </c>
       <c r="C61" t="s">
-        <v>512</v>
+        <v>119</v>
       </c>
       <c r="D61" t="s">
-        <v>513</v>
+        <v>378</v>
       </c>
       <c r="E61" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="F61" t="s">
-        <v>514</v>
-      </c>
-      <c r="G61" t="s">
-        <v>515</v>
+        <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -37125,22 +37134,19 @@
         <v>490</v>
       </c>
       <c r="B62" t="s">
-        <v>516</v>
+        <v>122</v>
       </c>
       <c r="C62" t="s">
-        <v>517</v>
+        <v>123</v>
       </c>
       <c r="D62" t="s">
-        <v>518</v>
+        <v>124</v>
       </c>
       <c r="E62" t="s">
-        <v>88</v>
+        <v>13</v>
       </c>
       <c r="F62" t="s">
-        <v>519</v>
-      </c>
-      <c r="G62" t="s">
-        <v>515</v>
+        <v>125</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -37148,22 +37154,19 @@
         <v>490</v>
       </c>
       <c r="B63" t="s">
-        <v>491</v>
+        <v>368</v>
       </c>
       <c r="C63" t="s">
-        <v>492</v>
+        <v>369</v>
       </c>
       <c r="D63" t="s">
-        <v>128</v>
+        <v>370</v>
       </c>
       <c r="E63" t="s">
-        <v>313</v>
+        <v>94</v>
       </c>
       <c r="F63" t="s">
-        <v>493</v>
-      </c>
-      <c r="G63" t="s">
-        <v>515</v>
+        <v>371</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -37171,22 +37174,19 @@
         <v>490</v>
       </c>
       <c r="B64" t="s">
-        <v>495</v>
+        <v>126</v>
       </c>
       <c r="C64" t="s">
-        <v>496</v>
+        <v>127</v>
       </c>
       <c r="D64" t="s">
-        <v>497</v>
+        <v>128</v>
       </c>
       <c r="E64" t="s">
-        <v>498</v>
+        <v>13</v>
       </c>
       <c r="F64" t="s">
-        <v>499</v>
-      </c>
-      <c r="G64" t="s">
-        <v>515</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -37194,22 +37194,19 @@
         <v>490</v>
       </c>
       <c r="B65" t="s">
-        <v>520</v>
+        <v>130</v>
       </c>
       <c r="C65" t="s">
-        <v>521</v>
+        <v>131</v>
       </c>
       <c r="D65" t="s">
-        <v>522</v>
+        <v>132</v>
       </c>
       <c r="E65" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="F65" t="s">
-        <v>522</v>
-      </c>
-      <c r="G65" t="s">
-        <v>515</v>
+        <v>376</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -37217,65 +37214,60 @@
         <v>490</v>
       </c>
       <c r="B66" t="s">
-        <v>523</v>
+        <v>310</v>
       </c>
       <c r="C66" t="s">
-        <v>524</v>
+        <v>311</v>
       </c>
       <c r="D66" t="s">
-        <v>525</v>
+        <v>312</v>
       </c>
       <c r="E66" t="s">
-        <v>142</v>
+        <v>313</v>
       </c>
       <c r="F66" t="s">
-        <v>525</v>
-      </c>
-      <c r="G66" t="s">
-        <v>515</v>
+        <v>314</v>
       </c>
     </row>
     <row r="67" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>490</v>
       </c>
-      <c r="B67" s="8" t="s">
-        <v>526</v>
-      </c>
-      <c r="C67" s="8" t="s">
-        <v>527</v>
-      </c>
-      <c r="D67" s="8" t="s">
-        <v>528</v>
-      </c>
-      <c r="E67" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="F67" s="8" t="s">
-        <v>528</v>
-      </c>
-      <c r="G67" t="s">
-        <v>515</v>
-      </c>
+      <c r="B67" t="s">
+        <v>468</v>
+      </c>
+      <c r="C67" t="s">
+        <v>469</v>
+      </c>
+      <c r="D67" t="s">
+        <v>380</v>
+      </c>
+      <c r="E67" t="s">
+        <v>76</v>
+      </c>
+      <c r="F67" t="s">
+        <v>381</v>
+      </c>
+      <c r="G67"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>490</v>
       </c>
       <c r="B68" t="s">
-        <v>436</v>
+        <v>468</v>
       </c>
       <c r="C68" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="D68" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="E68" t="s">
-        <v>439</v>
+        <v>25</v>
       </c>
       <c r="F68" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -37283,19 +37275,19 @@
         <v>490</v>
       </c>
       <c r="B69" t="s">
-        <v>146</v>
+        <v>468</v>
       </c>
       <c r="C69" t="s">
-        <v>441</v>
+        <v>215</v>
       </c>
       <c r="D69" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="E69" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="F69" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -37303,19 +37295,19 @@
         <v>490</v>
       </c>
       <c r="B70" t="s">
-        <v>468</v>
+        <v>404</v>
       </c>
       <c r="C70" t="s">
-        <v>475</v>
+        <v>405</v>
       </c>
       <c r="D70" t="s">
-        <v>442</v>
+        <v>406</v>
       </c>
       <c r="E70" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="F70" t="s">
-        <v>443</v>
+        <v>407</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -37323,39 +37315,45 @@
         <v>490</v>
       </c>
       <c r="B71" t="s">
-        <v>476</v>
+        <v>95</v>
       </c>
       <c r="C71" t="s">
-        <v>477</v>
+        <v>331</v>
       </c>
       <c r="D71" t="s">
-        <v>442</v>
+        <v>332</v>
       </c>
       <c r="E71" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F71" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+      <c r="G71" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="195" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>490</v>
       </c>
       <c r="B72" t="s">
-        <v>153</v>
+        <v>271</v>
       </c>
       <c r="C72" t="s">
-        <v>444</v>
+        <v>272</v>
       </c>
       <c r="D72" t="s">
-        <v>442</v>
+        <v>273</v>
       </c>
       <c r="E72" t="s">
-        <v>25</v>
+        <v>274</v>
       </c>
       <c r="F72" t="s">
-        <v>443</v>
+        <v>275</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -37363,19 +37361,19 @@
         <v>490</v>
       </c>
       <c r="B73" t="s">
-        <v>383</v>
+        <v>358</v>
       </c>
       <c r="C73" t="s">
-        <v>445</v>
+        <v>359</v>
       </c>
       <c r="D73" t="s">
-        <v>442</v>
+        <v>360</v>
       </c>
       <c r="E73" t="s">
-        <v>25</v>
+        <v>361</v>
       </c>
       <c r="F73" t="s">
-        <v>443</v>
+        <v>362</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -37383,19 +37381,22 @@
         <v>490</v>
       </c>
       <c r="B74" t="s">
-        <v>146</v>
+        <v>353</v>
       </c>
       <c r="C74" t="s">
-        <v>212</v>
+        <v>354</v>
       </c>
       <c r="D74" t="s">
-        <v>447</v>
+        <v>355</v>
       </c>
       <c r="E74" t="s">
-        <v>142</v>
+        <v>60</v>
       </c>
       <c r="F74" t="s">
-        <v>447</v>
+        <v>356</v>
+      </c>
+      <c r="G74" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -37403,19 +37404,19 @@
         <v>490</v>
       </c>
       <c r="B75" t="s">
-        <v>468</v>
+        <v>363</v>
       </c>
       <c r="C75" t="s">
-        <v>215</v>
+        <v>364</v>
       </c>
       <c r="D75" t="s">
-        <v>447</v>
+        <v>365</v>
       </c>
       <c r="E75" t="s">
         <v>142</v>
       </c>
       <c r="F75" t="s">
-        <v>447</v>
+        <v>365</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -37423,39 +37424,42 @@
         <v>490</v>
       </c>
       <c r="B76" t="s">
-        <v>476</v>
+        <v>366</v>
       </c>
       <c r="C76" t="s">
-        <v>529</v>
+        <v>367</v>
       </c>
       <c r="D76" t="s">
-        <v>447</v>
+        <v>365</v>
       </c>
       <c r="E76" t="s">
         <v>142</v>
       </c>
       <c r="F76" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>490</v>
       </c>
       <c r="B77" t="s">
-        <v>153</v>
+        <v>495</v>
       </c>
       <c r="C77" t="s">
-        <v>217</v>
+        <v>496</v>
       </c>
       <c r="D77" t="s">
-        <v>447</v>
+        <v>497</v>
       </c>
       <c r="E77" t="s">
-        <v>142</v>
+        <v>498</v>
       </c>
       <c r="F77" t="s">
-        <v>447</v>
+        <v>499</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -37463,19 +37467,22 @@
         <v>490</v>
       </c>
       <c r="B78" t="s">
-        <v>383</v>
+        <v>495</v>
       </c>
       <c r="C78" t="s">
-        <v>448</v>
+        <v>496</v>
       </c>
       <c r="D78" t="s">
-        <v>447</v>
+        <v>497</v>
       </c>
       <c r="E78" t="s">
-        <v>142</v>
+        <v>498</v>
       </c>
       <c r="F78" t="s">
-        <v>447</v>
+        <v>499</v>
+      </c>
+      <c r="G78" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -37483,22 +37490,19 @@
         <v>490</v>
       </c>
       <c r="B79" t="s">
-        <v>220</v>
+        <v>27</v>
       </c>
       <c r="C79" t="s">
-        <v>221</v>
+        <v>28</v>
       </c>
       <c r="D79" t="s">
-        <v>222</v>
+        <v>29</v>
       </c>
       <c r="E79" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="F79" t="s">
-        <v>222</v>
-      </c>
-      <c r="G79" t="s">
-        <v>223</v>
+        <v>30</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -37506,22 +37510,19 @@
         <v>490</v>
       </c>
       <c r="B80" t="s">
-        <v>224</v>
+        <v>31</v>
       </c>
       <c r="C80" t="s">
-        <v>225</v>
+        <v>304</v>
       </c>
       <c r="D80" t="s">
-        <v>450</v>
+        <v>305</v>
       </c>
       <c r="E80" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="F80" t="s">
-        <v>450</v>
-      </c>
-      <c r="G80" t="s">
-        <v>223</v>
+        <v>306</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -37529,26 +37530,30 @@
         <v>490</v>
       </c>
       <c r="B81" t="s">
-        <v>227</v>
+        <v>299</v>
       </c>
       <c r="C81" t="s">
-        <v>228</v>
+        <v>300</v>
       </c>
       <c r="D81" t="s">
-        <v>451</v>
+        <v>301</v>
       </c>
       <c r="E81" t="s">
-        <v>142</v>
+        <v>76</v>
       </c>
       <c r="F81" t="s">
-        <v>451</v>
+        <v>302</v>
       </c>
       <c r="G81" t="s">
-        <v>230</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G81" xr:uid="{F4D263A4-4B12-4751-864B-C8CA6DBD8F27}"/>
+  <autoFilter ref="A1:G81" xr:uid="{F4D263A4-4B12-4751-864B-C8CA6DBD8F27}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G81">
+      <sortCondition ref="B1:B81"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -37557,8 +37562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0700090A-CCDD-4BC5-A64F-4C0333BA8F70}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -37607,22 +37612,25 @@
         <v>532</v>
       </c>
       <c r="C2" t="s">
-        <v>255</v>
+        <v>282</v>
+      </c>
+      <c r="D2" t="s">
+        <v>283</v>
       </c>
       <c r="E2" t="s">
-        <v>256</v>
+        <v>284</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>247</v>
       </c>
       <c r="G2" t="s">
-        <v>257</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+      <c r="H2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2026</v>
       </c>
@@ -37630,22 +37638,25 @@
         <v>532</v>
       </c>
       <c r="C3" t="s">
-        <v>259</v>
+        <v>287</v>
+      </c>
+      <c r="D3" t="s">
+        <v>288</v>
       </c>
       <c r="E3" t="s">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>247</v>
       </c>
       <c r="G3" t="s">
-        <v>261</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>285</v>
+      </c>
+      <c r="H3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2026</v>
       </c>
@@ -37653,25 +37664,22 @@
         <v>532</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="E4" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2026</v>
       </c>
@@ -37679,25 +37687,22 @@
         <v>532</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="E5" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="F5" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2026</v>
       </c>
@@ -37705,25 +37710,25 @@
         <v>532</v>
       </c>
       <c r="C6" t="s">
-        <v>271</v>
+        <v>289</v>
       </c>
       <c r="D6" t="s">
-        <v>272</v>
+        <v>290</v>
       </c>
       <c r="E6" t="s">
-        <v>273</v>
+        <v>291</v>
       </c>
       <c r="F6" t="s">
-        <v>274</v>
+        <v>247</v>
       </c>
       <c r="G6" t="s">
-        <v>275</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="H6" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2026</v>
       </c>
@@ -37731,22 +37736,22 @@
         <v>532</v>
       </c>
       <c r="C7" t="s">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="D7" t="s">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="E7" t="s">
-        <v>279</v>
+        <v>295</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>247</v>
       </c>
       <c r="G7" t="s">
-        <v>280</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>281</v>
+        <v>296</v>
+      </c>
+      <c r="H7" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -37757,19 +37762,19 @@
         <v>532</v>
       </c>
       <c r="C8" t="s">
-        <v>282</v>
+        <v>297</v>
       </c>
       <c r="D8" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="E8" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="F8" t="s">
         <v>247</v>
       </c>
       <c r="G8" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
       <c r="H8" t="s">
         <v>286</v>
@@ -37783,25 +37788,22 @@
         <v>532</v>
       </c>
       <c r="C9" t="s">
-        <v>287</v>
+        <v>168</v>
       </c>
       <c r="D9" t="s">
-        <v>288</v>
+        <v>387</v>
       </c>
       <c r="E9" t="s">
-        <v>284</v>
+        <v>388</v>
       </c>
       <c r="F9" t="s">
-        <v>247</v>
+        <v>172</v>
       </c>
       <c r="G9" t="s">
-        <v>285</v>
-      </c>
-      <c r="H9" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2026</v>
       </c>
@@ -37809,22 +37811,22 @@
         <v>532</v>
       </c>
       <c r="C10" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="D10" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="E10" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
       <c r="F10" t="s">
-        <v>247</v>
+        <v>60</v>
       </c>
       <c r="G10" t="s">
-        <v>292</v>
-      </c>
-      <c r="H10" t="s">
-        <v>286</v>
+        <v>280</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -37835,22 +37837,19 @@
         <v>532</v>
       </c>
       <c r="C11" t="s">
-        <v>293</v>
+        <v>323</v>
       </c>
       <c r="D11" t="s">
-        <v>294</v>
+        <v>324</v>
       </c>
       <c r="E11" t="s">
-        <v>295</v>
+        <v>325</v>
       </c>
       <c r="F11" t="s">
-        <v>247</v>
+        <v>50</v>
       </c>
       <c r="G11" t="s">
-        <v>296</v>
-      </c>
-      <c r="H11" t="s">
-        <v>286</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -37861,22 +37860,19 @@
         <v>532</v>
       </c>
       <c r="C12" t="s">
-        <v>297</v>
+        <v>327</v>
       </c>
       <c r="D12" t="s">
-        <v>298</v>
+        <v>328</v>
       </c>
       <c r="E12" t="s">
-        <v>295</v>
+        <v>329</v>
       </c>
       <c r="F12" t="s">
-        <v>247</v>
+        <v>172</v>
       </c>
       <c r="G12" t="s">
-        <v>296</v>
-      </c>
-      <c r="H12" t="s">
-        <v>286</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -37887,22 +37883,19 @@
         <v>532</v>
       </c>
       <c r="C13" t="s">
-        <v>299</v>
+        <v>183</v>
       </c>
       <c r="D13" t="s">
-        <v>300</v>
+        <v>394</v>
       </c>
       <c r="E13" t="s">
-        <v>301</v>
+        <v>395</v>
       </c>
       <c r="F13" t="s">
-        <v>76</v>
+        <v>172</v>
       </c>
       <c r="G13" t="s">
-        <v>302</v>
-      </c>
-      <c r="H13" t="s">
-        <v>303</v>
+        <v>396</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -37913,19 +37906,19 @@
         <v>532</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>195</v>
       </c>
       <c r="D14" t="s">
-        <v>304</v>
+        <v>408</v>
       </c>
       <c r="E14" t="s">
-        <v>305</v>
+        <v>341</v>
       </c>
       <c r="F14" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="G14" t="s">
-        <v>306</v>
+        <v>409</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -37936,19 +37929,19 @@
         <v>532</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>410</v>
       </c>
       <c r="D15" t="s">
-        <v>28</v>
+        <v>411</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>412</v>
       </c>
       <c r="F15" t="s">
-        <v>13</v>
+        <v>172</v>
       </c>
       <c r="G15" t="s">
-        <v>30</v>
+        <v>413</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -37959,19 +37952,22 @@
         <v>532</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>424</v>
       </c>
       <c r="D16" t="s">
-        <v>307</v>
+        <v>425</v>
       </c>
       <c r="E16" t="s">
-        <v>308</v>
+        <v>406</v>
       </c>
       <c r="F16" t="s">
         <v>19</v>
       </c>
       <c r="G16" t="s">
-        <v>309</v>
+        <v>426</v>
+      </c>
+      <c r="H16" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -37982,19 +37978,22 @@
         <v>532</v>
       </c>
       <c r="C17" t="s">
-        <v>310</v>
+        <v>179</v>
       </c>
       <c r="D17" t="s">
-        <v>311</v>
+        <v>390</v>
       </c>
       <c r="E17" t="s">
-        <v>312</v>
+        <v>391</v>
       </c>
       <c r="F17" t="s">
-        <v>313</v>
+        <v>172</v>
       </c>
       <c r="G17" t="s">
-        <v>314</v>
+        <v>392</v>
+      </c>
+      <c r="H17" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -38005,22 +38004,22 @@
         <v>532</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>372</v>
       </c>
       <c r="D18" t="s">
-        <v>315</v>
+        <v>373</v>
       </c>
       <c r="E18" t="s">
-        <v>316</v>
+        <v>11</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="G18" t="s">
-        <v>317</v>
+        <v>374</v>
       </c>
       <c r="H18" t="s">
-        <v>318</v>
+        <v>375</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -38031,19 +38030,19 @@
         <v>532</v>
       </c>
       <c r="C19" t="s">
-        <v>319</v>
+        <v>153</v>
       </c>
       <c r="D19" t="s">
-        <v>320</v>
+        <v>382</v>
       </c>
       <c r="E19" t="s">
-        <v>321</v>
+        <v>380</v>
       </c>
       <c r="F19" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="G19" t="s">
-        <v>322</v>
+        <v>381</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -38054,19 +38053,19 @@
         <v>532</v>
       </c>
       <c r="C20" t="s">
-        <v>323</v>
+        <v>153</v>
       </c>
       <c r="D20" t="s">
-        <v>324</v>
+        <v>444</v>
       </c>
       <c r="E20" t="s">
-        <v>325</v>
+        <v>442</v>
       </c>
       <c r="F20" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="G20" t="s">
-        <v>326</v>
+        <v>443</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -38077,19 +38076,19 @@
         <v>532</v>
       </c>
       <c r="C21" t="s">
-        <v>327</v>
+        <v>153</v>
       </c>
       <c r="D21" t="s">
-        <v>328</v>
+        <v>217</v>
       </c>
       <c r="E21" t="s">
-        <v>329</v>
+        <v>447</v>
       </c>
       <c r="F21" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="G21" t="s">
-        <v>330</v>
+        <v>447</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -38100,22 +38099,22 @@
         <v>532</v>
       </c>
       <c r="C22" t="s">
-        <v>95</v>
+        <v>339</v>
       </c>
       <c r="D22" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="E22" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="G22" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="H22" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -38149,22 +38148,22 @@
         <v>532</v>
       </c>
       <c r="C24" t="s">
-        <v>339</v>
+        <v>191</v>
       </c>
       <c r="D24" t="s">
-        <v>340</v>
+        <v>400</v>
       </c>
       <c r="E24" t="s">
-        <v>341</v>
+        <v>401</v>
       </c>
       <c r="F24" t="s">
         <v>76</v>
       </c>
       <c r="G24" t="s">
-        <v>342</v>
+        <v>402</v>
       </c>
       <c r="H24" t="s">
-        <v>343</v>
+        <v>403</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -38175,19 +38174,19 @@
         <v>532</v>
       </c>
       <c r="C25" t="s">
-        <v>344</v>
+        <v>90</v>
       </c>
       <c r="D25" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="E25" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="F25" t="s">
         <v>94</v>
       </c>
       <c r="G25" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -38198,19 +38197,22 @@
         <v>532</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
+        <v>202</v>
       </c>
       <c r="D26" t="s">
-        <v>348</v>
+        <v>432</v>
       </c>
       <c r="E26" t="s">
-        <v>349</v>
+        <v>433</v>
       </c>
       <c r="F26" t="s">
-        <v>94</v>
+        <v>313</v>
       </c>
       <c r="G26" t="s">
-        <v>350</v>
+        <v>434</v>
+      </c>
+      <c r="H26" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -38221,19 +38223,22 @@
         <v>532</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="D27" t="s">
-        <v>351</v>
+        <v>315</v>
       </c>
       <c r="E27" t="s">
-        <v>132</v>
+        <v>316</v>
       </c>
       <c r="F27" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="G27" t="s">
-        <v>352</v>
+        <v>317</v>
+      </c>
+      <c r="H27" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -38244,19 +38249,22 @@
         <v>532</v>
       </c>
       <c r="C28" t="s">
-        <v>143</v>
+        <v>220</v>
       </c>
       <c r="D28" t="s">
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="E28" t="s">
-        <v>145</v>
+        <v>222</v>
       </c>
       <c r="F28" t="s">
         <v>142</v>
       </c>
       <c r="G28" t="s">
-        <v>145</v>
+        <v>222</v>
+      </c>
+      <c r="H28" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -38267,22 +38275,22 @@
         <v>532</v>
       </c>
       <c r="C29" t="s">
-        <v>353</v>
+        <v>224</v>
       </c>
       <c r="D29" t="s">
-        <v>354</v>
+        <v>225</v>
       </c>
       <c r="E29" t="s">
-        <v>355</v>
+        <v>450</v>
       </c>
       <c r="F29" t="s">
-        <v>60</v>
+        <v>142</v>
       </c>
       <c r="G29" t="s">
-        <v>356</v>
+        <v>450</v>
       </c>
       <c r="H29" t="s">
-        <v>357</v>
+        <v>223</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -38293,19 +38301,19 @@
         <v>532</v>
       </c>
       <c r="C30" t="s">
-        <v>358</v>
+        <v>319</v>
       </c>
       <c r="D30" t="s">
-        <v>359</v>
+        <v>320</v>
       </c>
       <c r="E30" t="s">
-        <v>360</v>
+        <v>321</v>
       </c>
       <c r="F30" t="s">
-        <v>361</v>
+        <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>362</v>
+        <v>322</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -38316,19 +38324,19 @@
         <v>532</v>
       </c>
       <c r="C31" t="s">
-        <v>363</v>
+        <v>143</v>
       </c>
       <c r="D31" t="s">
-        <v>364</v>
+        <v>144</v>
       </c>
       <c r="E31" t="s">
-        <v>365</v>
+        <v>145</v>
       </c>
       <c r="F31" t="s">
         <v>142</v>
       </c>
       <c r="G31" t="s">
-        <v>365</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -38339,19 +38347,19 @@
         <v>532</v>
       </c>
       <c r="C32" t="s">
-        <v>366</v>
+        <v>427</v>
       </c>
       <c r="D32" t="s">
-        <v>367</v>
+        <v>428</v>
       </c>
       <c r="E32" t="s">
-        <v>365</v>
+        <v>429</v>
       </c>
       <c r="F32" t="s">
-        <v>142</v>
+        <v>430</v>
       </c>
       <c r="G32" t="s">
-        <v>365</v>
+        <v>431</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -38362,19 +38370,19 @@
         <v>532</v>
       </c>
       <c r="C33" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="D33" t="s">
-        <v>369</v>
+        <v>345</v>
       </c>
       <c r="E33" t="s">
-        <v>370</v>
+        <v>346</v>
       </c>
       <c r="F33" t="s">
         <v>94</v>
       </c>
       <c r="G33" t="s">
-        <v>371</v>
+        <v>347</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -38385,22 +38393,22 @@
         <v>532</v>
       </c>
       <c r="C34" t="s">
-        <v>372</v>
+        <v>419</v>
       </c>
       <c r="D34" t="s">
-        <v>373</v>
+        <v>420</v>
       </c>
       <c r="E34" t="s">
-        <v>11</v>
+        <v>421</v>
       </c>
       <c r="F34" t="s">
-        <v>88</v>
+        <v>313</v>
       </c>
       <c r="G34" t="s">
-        <v>374</v>
+        <v>422</v>
       </c>
       <c r="H34" t="s">
-        <v>375</v>
+        <v>423</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -38411,19 +38419,22 @@
         <v>532</v>
       </c>
       <c r="C35" t="s">
-        <v>126</v>
+        <v>414</v>
       </c>
       <c r="D35" t="s">
-        <v>127</v>
+        <v>415</v>
       </c>
       <c r="E35" t="s">
-        <v>128</v>
+        <v>416</v>
       </c>
       <c r="F35" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="G35" t="s">
-        <v>129</v>
+        <v>417</v>
+      </c>
+      <c r="H35" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -38434,19 +38445,19 @@
         <v>532</v>
       </c>
       <c r="C36" t="s">
-        <v>130</v>
+        <v>72</v>
       </c>
       <c r="D36" t="s">
-        <v>131</v>
+        <v>307</v>
       </c>
       <c r="E36" t="s">
-        <v>132</v>
+        <v>308</v>
       </c>
       <c r="F36" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G36" t="s">
-        <v>376</v>
+        <v>309</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -38457,19 +38468,19 @@
         <v>532</v>
       </c>
       <c r="C37" t="s">
-        <v>377</v>
+        <v>476</v>
       </c>
       <c r="D37" t="s">
-        <v>110</v>
+        <v>480</v>
       </c>
       <c r="E37" t="s">
-        <v>111</v>
+        <v>380</v>
       </c>
       <c r="F37" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="G37" t="s">
-        <v>112</v>
+        <v>381</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -38480,19 +38491,19 @@
         <v>532</v>
       </c>
       <c r="C38" t="s">
-        <v>122</v>
+        <v>476</v>
       </c>
       <c r="D38" t="s">
-        <v>123</v>
+        <v>477</v>
       </c>
       <c r="E38" t="s">
-        <v>124</v>
+        <v>442</v>
       </c>
       <c r="F38" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="G38" t="s">
-        <v>125</v>
+        <v>443</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -38503,19 +38514,19 @@
         <v>532</v>
       </c>
       <c r="C39" t="s">
-        <v>118</v>
+        <v>476</v>
       </c>
       <c r="D39" t="s">
-        <v>119</v>
+        <v>529</v>
       </c>
       <c r="E39" t="s">
-        <v>378</v>
+        <v>447</v>
       </c>
       <c r="F39" t="s">
-        <v>13</v>
+        <v>142</v>
       </c>
       <c r="G39" t="s">
-        <v>121</v>
+        <v>447</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -38526,19 +38537,19 @@
         <v>532</v>
       </c>
       <c r="C40" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="D40" t="s">
-        <v>135</v>
+        <v>351</v>
       </c>
       <c r="E40" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F40" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="G40" t="s">
-        <v>137</v>
+        <v>352</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -38549,19 +38560,19 @@
         <v>532</v>
       </c>
       <c r="C41" t="s">
-        <v>146</v>
+        <v>206</v>
       </c>
       <c r="D41" t="s">
-        <v>379</v>
+        <v>207</v>
       </c>
       <c r="E41" t="s">
-        <v>380</v>
+        <v>435</v>
       </c>
       <c r="F41" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="G41" t="s">
-        <v>381</v>
+        <v>435</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -38572,19 +38583,19 @@
         <v>532</v>
       </c>
       <c r="C42" t="s">
-        <v>468</v>
+        <v>209</v>
       </c>
       <c r="D42" t="s">
-        <v>469</v>
+        <v>210</v>
       </c>
       <c r="E42" t="s">
-        <v>380</v>
+        <v>141</v>
       </c>
       <c r="F42" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="G42" t="s">
-        <v>381</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -38595,19 +38606,22 @@
         <v>532</v>
       </c>
       <c r="C43" t="s">
-        <v>476</v>
+        <v>227</v>
       </c>
       <c r="D43" t="s">
-        <v>480</v>
+        <v>228</v>
       </c>
       <c r="E43" t="s">
-        <v>380</v>
+        <v>451</v>
       </c>
       <c r="F43" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="G43" t="s">
-        <v>381</v>
+        <v>451</v>
+      </c>
+      <c r="H43" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -38618,19 +38632,19 @@
         <v>532</v>
       </c>
       <c r="C44" t="s">
-        <v>153</v>
+        <v>436</v>
       </c>
       <c r="D44" t="s">
-        <v>382</v>
+        <v>437</v>
       </c>
       <c r="E44" t="s">
-        <v>380</v>
+        <v>438</v>
       </c>
       <c r="F44" t="s">
-        <v>76</v>
+        <v>439</v>
       </c>
       <c r="G44" t="s">
-        <v>381</v>
+        <v>440</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -38641,10 +38655,10 @@
         <v>532</v>
       </c>
       <c r="C45" t="s">
-        <v>383</v>
+        <v>146</v>
       </c>
       <c r="D45" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="E45" t="s">
         <v>380</v>
@@ -38664,19 +38678,19 @@
         <v>532</v>
       </c>
       <c r="C46" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="D46" t="s">
-        <v>387</v>
+        <v>441</v>
       </c>
       <c r="E46" t="s">
-        <v>388</v>
+        <v>442</v>
       </c>
       <c r="F46" t="s">
-        <v>172</v>
+        <v>25</v>
       </c>
       <c r="G46" t="s">
-        <v>389</v>
+        <v>443</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -38687,25 +38701,22 @@
         <v>532</v>
       </c>
       <c r="C47" t="s">
-        <v>179</v>
+        <v>146</v>
       </c>
       <c r="D47" t="s">
-        <v>390</v>
+        <v>212</v>
       </c>
       <c r="E47" t="s">
-        <v>391</v>
+        <v>447</v>
       </c>
       <c r="F47" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="G47" t="s">
-        <v>392</v>
-      </c>
-      <c r="H47" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2026</v>
       </c>
@@ -38713,22 +38724,25 @@
         <v>532</v>
       </c>
       <c r="C48" t="s">
-        <v>183</v>
+        <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>394</v>
+        <v>263</v>
       </c>
       <c r="E48" t="s">
-        <v>395</v>
+        <v>264</v>
       </c>
       <c r="F48" t="s">
-        <v>172</v>
+        <v>13</v>
       </c>
       <c r="G48" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2026</v>
       </c>
@@ -38736,22 +38750,22 @@
         <v>532</v>
       </c>
       <c r="C49" t="s">
-        <v>187</v>
+        <v>15</v>
       </c>
       <c r="D49" t="s">
-        <v>397</v>
+        <v>267</v>
       </c>
       <c r="E49" t="s">
-        <v>398</v>
+        <v>268</v>
       </c>
       <c r="F49" t="s">
-        <v>13</v>
+        <v>94</v>
       </c>
       <c r="G49" t="s">
-        <v>399</v>
-      </c>
-      <c r="H49" t="s">
-        <v>393</v>
+        <v>269</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -38762,22 +38776,19 @@
         <v>532</v>
       </c>
       <c r="C50" t="s">
-        <v>191</v>
+        <v>383</v>
       </c>
       <c r="D50" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="E50" t="s">
-        <v>401</v>
+        <v>380</v>
       </c>
       <c r="F50" t="s">
         <v>76</v>
       </c>
       <c r="G50" t="s">
-        <v>402</v>
-      </c>
-      <c r="H50" t="s">
-        <v>403</v>
+        <v>381</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -38788,19 +38799,19 @@
         <v>532</v>
       </c>
       <c r="C51" t="s">
-        <v>404</v>
+        <v>383</v>
       </c>
       <c r="D51" t="s">
-        <v>405</v>
+        <v>445</v>
       </c>
       <c r="E51" t="s">
-        <v>406</v>
+        <v>442</v>
       </c>
       <c r="F51" t="s">
-        <v>94</v>
+        <v>25</v>
       </c>
       <c r="G51" t="s">
-        <v>407</v>
+        <v>443</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -38811,19 +38822,19 @@
         <v>532</v>
       </c>
       <c r="C52" t="s">
-        <v>195</v>
+        <v>383</v>
       </c>
       <c r="D52" t="s">
-        <v>408</v>
+        <v>448</v>
       </c>
       <c r="E52" t="s">
-        <v>341</v>
+        <v>447</v>
       </c>
       <c r="F52" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="G52" t="s">
-        <v>409</v>
+        <v>447</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -38834,19 +38845,22 @@
         <v>532</v>
       </c>
       <c r="C53" t="s">
-        <v>410</v>
+        <v>187</v>
       </c>
       <c r="D53" t="s">
-        <v>411</v>
+        <v>397</v>
       </c>
       <c r="E53" t="s">
-        <v>412</v>
+        <v>398</v>
       </c>
       <c r="F53" t="s">
-        <v>172</v>
+        <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>413</v>
+        <v>399</v>
+      </c>
+      <c r="H53" t="s">
+        <v>393</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -38857,22 +38871,19 @@
         <v>532</v>
       </c>
       <c r="C54" t="s">
-        <v>414</v>
+        <v>134</v>
       </c>
       <c r="D54" t="s">
-        <v>415</v>
+        <v>135</v>
       </c>
       <c r="E54" t="s">
-        <v>416</v>
+        <v>136</v>
       </c>
       <c r="F54" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G54" t="s">
-        <v>417</v>
-      </c>
-      <c r="H54" t="s">
-        <v>418</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -38883,22 +38894,19 @@
         <v>532</v>
       </c>
       <c r="C55" t="s">
-        <v>419</v>
+        <v>377</v>
       </c>
       <c r="D55" t="s">
-        <v>420</v>
+        <v>110</v>
       </c>
       <c r="E55" t="s">
-        <v>421</v>
+        <v>111</v>
       </c>
       <c r="F55" t="s">
-        <v>313</v>
+        <v>19</v>
       </c>
       <c r="G55" t="s">
-        <v>422</v>
-      </c>
-      <c r="H55" t="s">
-        <v>423</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -38909,22 +38917,19 @@
         <v>532</v>
       </c>
       <c r="C56" t="s">
-        <v>424</v>
+        <v>118</v>
       </c>
       <c r="D56" t="s">
-        <v>425</v>
+        <v>119</v>
       </c>
       <c r="E56" t="s">
-        <v>406</v>
+        <v>378</v>
       </c>
       <c r="F56" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="G56" t="s">
-        <v>426</v>
-      </c>
-      <c r="H56" t="s">
-        <v>393</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -38935,19 +38940,19 @@
         <v>532</v>
       </c>
       <c r="C57" t="s">
-        <v>427</v>
+        <v>122</v>
       </c>
       <c r="D57" t="s">
-        <v>428</v>
+        <v>123</v>
       </c>
       <c r="E57" t="s">
-        <v>429</v>
+        <v>124</v>
       </c>
       <c r="F57" t="s">
-        <v>430</v>
+        <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>431</v>
+        <v>125</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -38958,22 +38963,19 @@
         <v>532</v>
       </c>
       <c r="C58" t="s">
-        <v>202</v>
+        <v>368</v>
       </c>
       <c r="D58" t="s">
-        <v>432</v>
+        <v>369</v>
       </c>
       <c r="E58" t="s">
-        <v>433</v>
+        <v>370</v>
       </c>
       <c r="F58" t="s">
-        <v>313</v>
+        <v>94</v>
       </c>
       <c r="G58" t="s">
-        <v>434</v>
-      </c>
-      <c r="H58" t="s">
-        <v>393</v>
+        <v>371</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -38984,19 +38986,19 @@
         <v>532</v>
       </c>
       <c r="C59" t="s">
-        <v>206</v>
+        <v>126</v>
       </c>
       <c r="D59" t="s">
-        <v>207</v>
+        <v>127</v>
       </c>
       <c r="E59" t="s">
-        <v>435</v>
+        <v>128</v>
       </c>
       <c r="F59" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="G59" t="s">
-        <v>435</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -39007,19 +39009,19 @@
         <v>532</v>
       </c>
       <c r="C60" t="s">
-        <v>209</v>
+        <v>130</v>
       </c>
       <c r="D60" t="s">
-        <v>210</v>
+        <v>131</v>
       </c>
       <c r="E60" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F60" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="G60" t="s">
-        <v>141</v>
+        <v>376</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -39030,19 +39032,19 @@
         <v>532</v>
       </c>
       <c r="C61" t="s">
-        <v>436</v>
+        <v>310</v>
       </c>
       <c r="D61" t="s">
-        <v>437</v>
+        <v>311</v>
       </c>
       <c r="E61" t="s">
-        <v>438</v>
+        <v>312</v>
       </c>
       <c r="F61" t="s">
-        <v>439</v>
+        <v>313</v>
       </c>
       <c r="G61" t="s">
-        <v>440</v>
+        <v>314</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -39053,19 +39055,19 @@
         <v>532</v>
       </c>
       <c r="C62" t="s">
-        <v>146</v>
+        <v>468</v>
       </c>
       <c r="D62" t="s">
-        <v>441</v>
+        <v>469</v>
       </c>
       <c r="E62" t="s">
-        <v>442</v>
+        <v>380</v>
       </c>
       <c r="F62" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="G62" t="s">
-        <v>443</v>
+        <v>381</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -39099,19 +39101,19 @@
         <v>532</v>
       </c>
       <c r="C64" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="D64" t="s">
-        <v>477</v>
+        <v>215</v>
       </c>
       <c r="E64" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="F64" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
       <c r="G64" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -39122,19 +39124,19 @@
         <v>532</v>
       </c>
       <c r="C65" t="s">
-        <v>153</v>
+        <v>404</v>
       </c>
       <c r="D65" t="s">
-        <v>444</v>
+        <v>405</v>
       </c>
       <c r="E65" t="s">
-        <v>442</v>
+        <v>406</v>
       </c>
       <c r="F65" t="s">
-        <v>25</v>
+        <v>94</v>
       </c>
       <c r="G65" t="s">
-        <v>443</v>
+        <v>407</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -39145,22 +39147,25 @@
         <v>532</v>
       </c>
       <c r="C66" t="s">
-        <v>383</v>
+        <v>95</v>
       </c>
       <c r="D66" t="s">
-        <v>445</v>
+        <v>331</v>
       </c>
       <c r="E66" t="s">
-        <v>442</v>
+        <v>332</v>
       </c>
       <c r="F66" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G66" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+        <v>333</v>
+      </c>
+      <c r="H66" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2026</v>
       </c>
@@ -39168,19 +39173,22 @@
         <v>532</v>
       </c>
       <c r="C67" t="s">
-        <v>146</v>
+        <v>271</v>
       </c>
       <c r="D67" t="s">
-        <v>212</v>
+        <v>272</v>
       </c>
       <c r="E67" t="s">
-        <v>447</v>
+        <v>273</v>
       </c>
       <c r="F67" t="s">
-        <v>142</v>
+        <v>274</v>
       </c>
       <c r="G67" t="s">
-        <v>447</v>
+        <v>275</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -39191,19 +39199,19 @@
         <v>532</v>
       </c>
       <c r="C68" t="s">
-        <v>468</v>
+        <v>358</v>
       </c>
       <c r="D68" t="s">
-        <v>215</v>
+        <v>359</v>
       </c>
       <c r="E68" t="s">
-        <v>447</v>
+        <v>360</v>
       </c>
       <c r="F68" t="s">
-        <v>142</v>
+        <v>361</v>
       </c>
       <c r="G68" t="s">
-        <v>447</v>
+        <v>362</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -39214,19 +39222,22 @@
         <v>532</v>
       </c>
       <c r="C69" t="s">
-        <v>476</v>
+        <v>353</v>
       </c>
       <c r="D69" t="s">
-        <v>529</v>
+        <v>354</v>
       </c>
       <c r="E69" t="s">
-        <v>447</v>
+        <v>355</v>
       </c>
       <c r="F69" t="s">
-        <v>142</v>
+        <v>60</v>
       </c>
       <c r="G69" t="s">
-        <v>447</v>
+        <v>356</v>
+      </c>
+      <c r="H69" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -39237,19 +39248,19 @@
         <v>532</v>
       </c>
       <c r="C70" t="s">
-        <v>153</v>
+        <v>363</v>
       </c>
       <c r="D70" t="s">
-        <v>217</v>
+        <v>364</v>
       </c>
       <c r="E70" t="s">
-        <v>447</v>
+        <v>365</v>
       </c>
       <c r="F70" t="s">
         <v>142</v>
       </c>
       <c r="G70" t="s">
-        <v>447</v>
+        <v>365</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -39260,19 +39271,19 @@
         <v>532</v>
       </c>
       <c r="C71" t="s">
-        <v>383</v>
+        <v>366</v>
       </c>
       <c r="D71" t="s">
-        <v>448</v>
+        <v>367</v>
       </c>
       <c r="E71" t="s">
-        <v>447</v>
+        <v>365</v>
       </c>
       <c r="F71" t="s">
         <v>142</v>
       </c>
       <c r="G71" t="s">
-        <v>447</v>
+        <v>365</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
@@ -39283,22 +39294,19 @@
         <v>532</v>
       </c>
       <c r="C72" t="s">
-        <v>220</v>
+        <v>27</v>
       </c>
       <c r="D72" t="s">
-        <v>221</v>
+        <v>28</v>
       </c>
       <c r="E72" t="s">
-        <v>222</v>
+        <v>29</v>
       </c>
       <c r="F72" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="G72" t="s">
-        <v>222</v>
-      </c>
-      <c r="H72" t="s">
-        <v>223</v>
+        <v>30</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
@@ -39309,22 +39317,19 @@
         <v>532</v>
       </c>
       <c r="C73" t="s">
-        <v>224</v>
+        <v>31</v>
       </c>
       <c r="D73" t="s">
-        <v>225</v>
+        <v>304</v>
       </c>
       <c r="E73" t="s">
-        <v>450</v>
+        <v>305</v>
       </c>
       <c r="F73" t="s">
-        <v>142</v>
+        <v>13</v>
       </c>
       <c r="G73" t="s">
-        <v>450</v>
-      </c>
-      <c r="H73" t="s">
-        <v>223</v>
+        <v>306</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -39335,26 +39340,30 @@
         <v>532</v>
       </c>
       <c r="C74" t="s">
-        <v>227</v>
+        <v>299</v>
       </c>
       <c r="D74" t="s">
-        <v>228</v>
+        <v>300</v>
       </c>
       <c r="E74" t="s">
-        <v>451</v>
+        <v>301</v>
       </c>
       <c r="F74" t="s">
-        <v>142</v>
+        <v>76</v>
       </c>
       <c r="G74" t="s">
-        <v>451</v>
+        <v>302</v>
       </c>
       <c r="H74" t="s">
-        <v>230</v>
+        <v>303</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:H74" xr:uid="{0700090A-CCDD-4BC5-A64F-4C0333BA8F70}"/>
+  <autoFilter ref="B1:H74" xr:uid="{0700090A-CCDD-4BC5-A64F-4C0333BA8F70}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:H74">
+      <sortCondition ref="C1:C74"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -43265,9 +43274,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F2E6FD5-1122-431F-B0AF-A11DEA581360}">
   <dimension ref="A1:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>